<commit_message>
Updated the syllabus for F24
</commit_message>
<xml_diff>
--- a/WeekDates.xlsx
+++ b/WeekDates.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D07F0B3-1487-4D7A-AA11-E6771D2C7029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A82073-4240-0F45-8774-64B0173E3659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20364" yWindow="5280" windowWidth="17556" windowHeight="10080" xr2:uid="{51C34D7A-4123-40D0-B0D1-4F8A4C5B2950}"/>
+    <workbookView xWindow="15600" yWindow="500" windowWidth="10000" windowHeight="14520" xr2:uid="{51C34D7A-4123-40D0-B0D1-4F8A4C5B2950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,25 +37,209 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Week</t>
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Intro to JavaScript:</t>
+  </si>
+  <si>
+    <t>algorithms, variables, and data types</t>
+  </si>
+  <si>
+    <t>Reading quiz 1</t>
+  </si>
+  <si>
+    <t>Beta version of lab 1</t>
+  </si>
+  <si>
+    <t>Functions, Expressions and Operators</t>
+  </si>
+  <si>
+    <t>Reading quiz 2 </t>
+  </si>
+  <si>
+    <t>Production version of lab 1</t>
+  </si>
+  <si>
+    <t>Beta version of lab 2</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>lab 2 code review </t>
+  </si>
+  <si>
+    <t>Reading quiz 3 </t>
+  </si>
+  <si>
+    <t>Production version of lab 2 </t>
+  </si>
+  <si>
+    <t>Beta version of lab 3</t>
+  </si>
+  <si>
+    <t>Repetition</t>
+  </si>
+  <si>
+    <t>lab 3 code review</t>
+  </si>
+  <si>
+    <t>Reading quiz 4</t>
+  </si>
+  <si>
+    <t>Production version of lab 3</t>
+  </si>
+  <si>
+    <t>Beta version of lab 4</t>
+  </si>
+  <si>
+    <t>Midterm Check-Point</t>
+  </si>
+  <si>
+    <t>lab 4 code review </t>
+  </si>
+  <si>
+    <t>Production version of lab 4 </t>
+  </si>
+  <si>
+    <t>Term project proposal</t>
+  </si>
+  <si>
+    <t>Midterm quiz:</t>
+  </si>
+  <si>
+    <t>- In the classroom at 12:00 on 5/3</t>
+  </si>
+  <si>
+    <t>- In the testing center 5/3 or 5/4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Reading quiz 5 </t>
+  </si>
+  <si>
+    <t>Beta version of lab 5</t>
+  </si>
+  <si>
+    <t>Objects</t>
+  </si>
+  <si>
+    <t>lab 5 code review</t>
+  </si>
+  <si>
+    <t>Reading quiz 6</t>
+  </si>
+  <si>
+    <t>Production version of lab 5</t>
+  </si>
+  <si>
+    <t>Beta version of lab 6</t>
+  </si>
+  <si>
+    <t>Document Object Model and Events</t>
+  </si>
+  <si>
+    <t>lab 6 code review</t>
+  </si>
+  <si>
+    <t>Reading quiz 7</t>
+  </si>
+  <si>
+    <t>Production version of lab 6</t>
+  </si>
+  <si>
+    <t>Beta version of lab 7</t>
+  </si>
+  <si>
+    <t>Monday: Memorial Day Holiday</t>
+  </si>
+  <si>
+    <t>Regular Expressions</t>
+  </si>
+  <si>
+    <t>lab 7 code review</t>
+  </si>
+  <si>
+    <t>Reading quiz 8</t>
+  </si>
+  <si>
+    <t>Production version of lab 7</t>
+  </si>
+  <si>
+    <t>Beta version of lab 8</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Term project</t>
+  </si>
+  <si>
+    <t>Extra credit lab</t>
+  </si>
+  <si>
+    <t>Finals week</t>
+  </si>
+  <si>
+    <t>Final quiz</t>
+  </si>
+  <si>
+    <t>- In the classroom at 12:00 6/12</t>
+  </si>
+  <si>
+    <t>- In the testing center 6/12—6/14</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>lab 1 code review
+Reading quiz 2 
+Production version of lab 1
+Beta version of lab 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="m/d;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,9 +262,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,9 +293,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +333,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -244,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,16 +591,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34FAE36-92AF-4168-8147-1C71401B1149}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,96 +608,490 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>45019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>45026</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <f>B2+7</f>
+        <v>45572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>45033</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" ref="B4:B12" si="0">B3+7</f>
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>45040</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>45047</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>45054</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>45061</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45607</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>45068</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45614</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>45075</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>45082</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>45628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>45089</v>
+        <f t="shared" si="0"/>
+        <v>45635</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319C4403-4CBE-904C-8DE2-48747A2D0311}">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" customWidth="1"/>
+    <col min="3" max="3" width="47.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>45565</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="104" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f>A3+7</f>
+        <v>45572</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f>A5+7</f>
+        <v>45579</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f>A9+7</f>
+        <v>45586</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f>A13+7</f>
+        <v>45593</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <f>A17+7</f>
+        <v>45600</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <f>A23+7</f>
+        <v>45607</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f>A25+7</f>
+        <v>45614</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <f>A29+7</f>
+        <v>45621</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <f>A33+7</f>
+        <v>45628</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="26" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>11</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <f>A37+7</f>
+        <v>45635</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="52" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished updating the syllabus
</commit_message>
<xml_diff>
--- a/WeekDates.xlsx
+++ b/WeekDates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A82073-4240-0F45-8774-64B0173E3659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC95A31-B5D9-844F-97D3-83D0B8801B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="500" windowWidth="10000" windowHeight="14520" xr2:uid="{51C34D7A-4123-40D0-B0D1-4F8A4C5B2950}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14520" activeTab="1" xr2:uid="{51C34D7A-4123-40D0-B0D1-4F8A4C5B2950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
   <si>
     <t>Week</t>
   </si>
@@ -117,12 +117,6 @@
     <t>Midterm quiz:</t>
   </si>
   <si>
-    <t>- In the classroom at 12:00 on 5/3</t>
-  </si>
-  <si>
-    <t>- In the testing center 5/3 or 5/4</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>Beta version of lab 7</t>
   </si>
   <si>
-    <t>Monday: Memorial Day Holiday</t>
-  </si>
-  <si>
     <t>Regular Expressions</t>
   </si>
   <si>
@@ -186,9 +177,6 @@
     <t>Review</t>
   </si>
   <si>
-    <t>Term project</t>
-  </si>
-  <si>
     <t>Extra credit lab</t>
   </si>
   <si>
@@ -198,19 +186,52 @@
     <t>Final quiz</t>
   </si>
   <si>
-    <t>- In the classroom at 12:00 6/12</t>
-  </si>
-  <si>
-    <t>- In the testing center 6/12—6/14</t>
-  </si>
-  <si>
     <t>Due</t>
   </si>
   <si>
-    <t>lab 1 code review
-Reading quiz 2 
-Production version of lab 1
-Beta version of lab 2</t>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>lab 1 code review</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>- In the classroom</t>
+  </si>
+  <si>
+    <t>- In the testing center 10/31, 9am--11/2, 5pm?</t>
+  </si>
+  <si>
+    <t>- In the testing center 12/10, 9am--12/12, 7:30pm</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Production version of lab 8</t>
+  </si>
+  <si>
+    <t>Lab 8 code review</t>
+  </si>
+  <si>
+    <t>Beta version of term project</t>
+  </si>
+  <si>
+    <t>Term project code review</t>
+  </si>
+  <si>
+    <t>Term project production versioin</t>
   </si>
 </sst>
 </file>
@@ -220,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="169" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +262,13 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +278,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -258,26 +286,176 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -591,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34FAE36-92AF-4168-8147-1C71401B1149}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -714,382 +892,707 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319C4403-4CBE-904C-8DE2-48747A2D0311}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="3" width="47.5" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7">
+        <f>A3+2</f>
+        <v>45567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="53" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
+        <v>45565</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="14">
+        <f>A3+4</f>
+        <v>45569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="53" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>45565</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="104" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E4" s="7">
+        <f>A5</f>
+        <v>45572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <f>A3+7</f>
         <v>45572</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="D5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="11">
+        <f>A5+2</f>
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="D6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="11">
+        <f>A5+3</f>
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="D7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="14">
+        <f>A5+4</f>
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="D8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="7">
+        <f>A9</f>
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <f>A5+7</f>
         <v>45579</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="D9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="11">
+        <f>A9+2</f>
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="D10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="11">
+        <f>A9+3</f>
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="D11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="14">
+        <f>A9+4</f>
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>4</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="7">
+        <f>A13+2</f>
+        <v>45588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <f>A9+7</f>
         <v>45586</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="D13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="11">
+        <f>A13+2</f>
+        <v>45588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="D14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="11">
+        <f>A13+3</f>
+        <v>45589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="D15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="14">
+        <f>A13+4</f>
+        <v>45590</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="D16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="7">
+        <f>A17</f>
+        <v>45593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
         <f>A13+7</f>
         <v>45593</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
+      <c r="D17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="11">
+        <f>A17+3</f>
+        <v>45596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+      <c r="D18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="11">
+        <f>A17+3</f>
+        <v>45596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="D19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="11">
+        <f>A17+3</f>
+        <v>45596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="11">
+        <v>45596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="53" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="D22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="7">
+        <f>A23+2</f>
+        <v>45602</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A23" s="17">
         <f>A17+7</f>
         <v>45600</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="14">
+        <f>A23+4</f>
+        <v>45604</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>7</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="D24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="7">
+        <f>A25</f>
+        <v>45607</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
         <f>A23+7</f>
         <v>45607</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="23">
+        <f>A25+2</f>
+        <v>45609</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="11">
+        <f>A25+3</f>
+        <v>45610</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="D27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="14">
+        <f>A25+4</f>
+        <v>45611</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="53" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>8</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="D28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="7">
+        <f>A29</f>
+        <v>45614</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
         <f>A25+7</f>
         <v>45614</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="11">
+        <f>A29+2</f>
+        <v>45616</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="11">
+        <f>A29+3</f>
+        <v>45617</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="14">
+        <f>A29+4</f>
+        <v>45618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>9</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>9</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="D32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="7">
+        <f>A33</f>
+        <v>45621</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
         <f>A29+7</f>
         <v>45621</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="11">
+        <f>A33+2</f>
+        <v>45623</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A34" s="15"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D34" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="11">
+        <f>A33+3</f>
+        <v>45624</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="14">
+        <f>A33+4</f>
+        <v>45625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>10</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>10</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="C36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="7">
+        <f>A37</f>
+        <v>45628</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
         <f>A33+7</f>
         <v>45628</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="26" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="E37" s="11">
+        <f>A37+4</f>
+        <v>45632</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="11">
+        <f>A37+4</f>
+        <v>45632</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="11">
+        <f>A37+6</f>
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
         <v>11</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="B40" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="7">
+        <f>A41+1</f>
+        <v>45636</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
         <f>A37+7</f>
         <v>45635</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="52" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
+      <c r="B41" s="24"/>
+      <c r="C41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="E41" s="7">
+        <f>A41+1</f>
+        <v>45636</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="11">
+        <v>45636</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="B43" s="24"/>
+      <c r="C43" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="25"/>
+    </row>
+    <row r="44" spans="1:5" ht="53" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="13"/>
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="B46" s="24"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="D48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>